<commit_message>
Added lotsa shit yo
</commit_message>
<xml_diff>
--- a/Lab4/Average_Times.xlsx
+++ b/Lab4/Average_Times.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="8310" windowHeight="2580" xr2:uid="{B17AB255-5C8A-4D10-BD93-206132F9DB2D}"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="8310" windowHeight="2580" xr2:uid="{B17AB255-5C8A-4D10-BD93-206132F9DB2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Avg</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -370,31 +384,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40FA358B-CFC2-4ACC-A981-36F1CD55E796}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>21026510</v>
       </c>
       <c r="C1">
         <v>31200196</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>6606986</v>
       </c>
       <c r="C2">
         <v>21895502</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <f>MIN(A1:A10)/200000000*1000</f>
+        <v>32.269289999999998</v>
+      </c>
+      <c r="F2">
+        <f>MIN(C1:C10)/200000000*1000</f>
+        <v>76.593360000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>15633272</v>
       </c>
@@ -402,23 +427,34 @@
         <v>33398226</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6531454</v>
       </c>
       <c r="C4">
         <v>58153518</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9784206</v>
       </c>
       <c r="C5">
         <v>38155744</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <f>MAX(A1:A10)/200000000*1000</f>
+        <v>105.13255000000001</v>
+      </c>
+      <c r="F5">
+        <f>MAX(C1:C10)/200000000*1000</f>
+        <v>290.76759000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6902470</v>
       </c>
@@ -426,23 +462,34 @@
         <v>16527664</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6453858</v>
       </c>
       <c r="C7">
         <v>33031274</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>11764512</v>
       </c>
       <c r="C8">
         <v>15318672</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <f>AVERAGE(A1:A10)/200000000*1000</f>
+        <v>50.402707999999997</v>
+      </c>
+      <c r="F8">
+        <f>AVERAGE(C1:C10)/200000000*1000</f>
+        <v>152.61173099999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9311696</v>
       </c>
@@ -450,7 +497,7 @@
         <v>36079992</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6790452</v>
       </c>
@@ -458,13 +505,8 @@
         <v>21462674</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C11">
-        <f>AVERAGE(C1:C10)/200000000</f>
-        <v>0.152611731</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>